<commit_message>
Edit CD method create_token
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -185,20 +185,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>44734</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:colOff>306135</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -211,8 +211,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="571500"/>
-          <a:ext cx="11017534" cy="10572749"/>
+          <a:off x="628651" y="390524"/>
+          <a:ext cx="10650284" cy="10220325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -489,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G22" workbookViewId="0">
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update API Design and unit testting code for create user ver 1
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\blog\doc\API_Design\API_Detail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\_blog\blog\doc\API_Design\API_Detail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -185,20 +185,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>200024</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>306135</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>157649</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -211,8 +211,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="628651" y="390524"/>
-          <a:ext cx="10650284" cy="10220325"/>
+          <a:off x="9525" y="619124"/>
+          <a:ext cx="10511324" cy="10086975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G22" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Design for login function
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -186,19 +186,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>157649</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>20751</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -211,8 +211,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525" y="619124"/>
-          <a:ext cx="10511324" cy="10086975"/>
+          <a:off x="0" y="409574"/>
+          <a:ext cx="11603151" cy="11134725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
Update API Design detail : flow,SD,CD,Spec for login function
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\blog\doc\API_Design\API_Detail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\_blog\blog\doc\API_Design\API_Detail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -185,20 +185,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>200024</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>306135</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>20751</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -211,8 +211,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="628651" y="390524"/>
-          <a:ext cx="10650284" cy="10220325"/>
+          <a:off x="0" y="409574"/>
+          <a:ext cx="11603151" cy="11134725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G22" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update CD for user logout
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -186,20 +186,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>216185</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -212,8 +212,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1390650" y="381000"/>
-          <a:ext cx="11017535" cy="10572750"/>
+          <a:off x="609600" y="581025"/>
+          <a:ext cx="14392275" cy="13811250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -490,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add function get user by token to get info user current login
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -186,20 +186,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>539818</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -212,8 +212,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="581025"/>
-          <a:ext cx="14392275" cy="13811250"/>
+          <a:off x="28575" y="533399"/>
+          <a:ext cx="11484043" cy="11020425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
Edit error code in Spec, edit Flow, CD
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
-    <sheet name="Register user" sheetId="1" r:id="rId1"/>
+    <sheet name="System CD" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>REGISTER USER CLASS DIAGRAM</t>
+    <t>SYSTEM CLASS DIAGRAM</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update funciton validate_update to validate lastname,firstname,email updated
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -187,19 +187,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>539818</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>388003</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -212,8 +212,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28575" y="533399"/>
-          <a:ext cx="11484043" cy="11020425"/>
+          <a:off x="0" y="476250"/>
+          <a:ext cx="11970403" cy="11487150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Edit Flow, CD, Spec check token return user id , update user uby user id
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -187,19 +187,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>388003</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>350428</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -212,8 +212,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="476250"/>
-          <a:ext cx="11970403" cy="11487150"/>
+          <a:off x="47625" y="400050"/>
+          <a:ext cx="11275603" cy="10820400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -490,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Upload design for get user info
</commit_message>
<xml_diff>
--- a/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
+++ b/doc/API_Design/API_Detail/BLOG_API_CD.xlsx
@@ -187,19 +187,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>66676</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>350428</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>326451</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -212,8 +212,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="47625" y="400050"/>
-          <a:ext cx="11275603" cy="10820400"/>
+          <a:off x="66676" y="419100"/>
+          <a:ext cx="8794175" cy="8439149"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>